<commit_message>
started on the function to create database
</commit_message>
<xml_diff>
--- a/data structure plan.xlsx
+++ b/data structure plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Programs\3DS Pokedex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{949F3544-B383-4CCE-81D6-0034754F720B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8DE223-72BA-489E-AAD3-9682FCC2BA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{E8F28A6F-6F1D-4032-9281-A373BEA9A053}"/>
+    <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{E8F28A6F-6F1D-4032-9281-A373BEA9A053}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -625,9 +625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31FDE52E-1438-4E4D-B985-58AEBB556F45}">
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>

</xml_diff>

<commit_message>
just final update to strucutre plan
</commit_message>
<xml_diff>
--- a/data structure plan.xlsx
+++ b/data structure plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Programs\3DS Pokedex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8DE223-72BA-489E-AAD3-9682FCC2BA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06DC0C9-E588-40F9-ACA8-EAA4B77636FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{E8F28A6F-6F1D-4032-9281-A373BEA9A053}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{E8F28A6F-6F1D-4032-9281-A373BEA9A053}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -224,9 +224,6 @@
     <t>List of Pokemon it evolves into: Method (1 byte) target (2) method (2) forme target (1) number parameter (1)</t>
   </si>
   <si>
-    <t>List of egg moves Move (2 bytes) each</t>
-  </si>
-  <si>
     <t>List of evolves into it: source (2) forme (1) Method (1 byte) method (2)  number parameter (1)</t>
   </si>
   <si>
@@ -249,6 +246,9 @@
   </si>
   <si>
     <t>internal personal #</t>
+  </si>
+  <si>
+    <t>List of egg moves Move index (2 bytes) each</t>
   </si>
 </sst>
 </file>
@@ -623,39 +623,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31FDE52E-1438-4E4D-B985-58AEBB556F45}">
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="83.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="D1">
-        <f>SUM(C:C)</f>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <f>A2+1</f>
         <v>1</v>
@@ -667,7 +665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <f t="shared" ref="A4:A66" si="0">A3+1</f>
         <v>2</v>
@@ -679,19 +677,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -703,31 +701,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>69</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>70</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -739,7 +737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -751,7 +749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -763,7 +761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -775,7 +773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -787,7 +785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -799,7 +797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -811,7 +809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1444,26 +1442,24 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B67" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="C67" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B68" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B69" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B70" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixes to egg move handling
</commit_message>
<xml_diff>
--- a/data structure plan.xlsx
+++ b/data structure plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Programs\3DS Pokedex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06DC0C9-E588-40F9-ACA8-EAA4B77636FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66F0BD5-B535-489C-ABEB-9402FA48014B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{E8F28A6F-6F1D-4032-9281-A373BEA9A053}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Pokemon Data Structure</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>List of egg moves Move index (2 bytes) each</t>
+  </si>
+  <si>
+    <t># levelup moves</t>
+  </si>
+  <si>
+    <t>bytes per entry frome here on</t>
   </si>
 </sst>
 </file>
@@ -623,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31FDE52E-1438-4E4D-B985-58AEBB556F45}">
-  <dimension ref="A1:K69"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -667,7 +673,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
-        <f t="shared" ref="A4:A66" si="0">A3+1</f>
+        <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -695,10 +701,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -707,10 +713,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -719,10 +725,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -731,10 +737,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -743,7 +749,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -755,7 +761,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -767,7 +773,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -779,7 +785,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -791,7 +797,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -803,7 +809,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -815,7 +821,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -827,7 +833,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -839,7 +845,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -851,14 +857,11 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="2"/>
-      <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20">
@@ -866,7 +869,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -881,7 +884,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -896,7 +899,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -911,7 +914,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -926,10 +929,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="2"/>
@@ -941,7 +944,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -956,7 +959,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -971,10 +974,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="2"/>
@@ -986,11 +989,14 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="2"/>
+      <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29">
@@ -998,7 +1004,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1010,7 +1016,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1022,7 +1028,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1034,7 +1040,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1046,7 +1052,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1058,7 +1064,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -1070,7 +1076,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1082,7 +1088,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1094,7 +1100,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1106,7 +1112,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -1118,7 +1124,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -1130,7 +1136,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -1142,7 +1148,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -1154,7 +1160,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -1166,7 +1172,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1178,7 +1184,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -1190,7 +1196,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -1202,7 +1208,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1214,7 +1220,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -1226,7 +1232,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -1238,7 +1244,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -1250,7 +1256,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -1262,7 +1268,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -1274,7 +1280,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -1286,7 +1292,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -1298,7 +1304,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1310,7 +1316,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -1322,7 +1328,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -1334,7 +1340,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -1346,7 +1352,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -1358,7 +1364,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -1370,7 +1376,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -1382,10 +1388,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
@@ -1394,7 +1400,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C62">
         <v>2</v>
@@ -1406,7 +1412,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C63">
         <v>2</v>
@@ -1418,49 +1424,81 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C64">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C65">
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="B66" t="s">
+        <v>53</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B67" t="s">
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B68" t="s">
         <v>61</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B69" t="s">
+        <v>62</v>
+      </c>
+      <c r="C69">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B70" t="s">
+        <v>63</v>
+      </c>
+      <c r="C70">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B71" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B68" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B69" t="s">
-        <v>63</v>
+      <c r="C71">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix to recursion and evolution implementation
</commit_message>
<xml_diff>
--- a/data structure plan.xlsx
+++ b/data structure plan.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Programs\3DS Pokedex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66F0BD5-B535-489C-ABEB-9402FA48014B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F76F4D4-AFAE-4FA2-B427-56E885CAFE50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{E8F28A6F-6F1D-4032-9281-A373BEA9A053}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Evolution" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="141">
   <si>
     <t>Pokemon Data Structure</t>
   </si>
@@ -221,12 +222,6 @@
     <t>List of levelup moves Move (2 bytes) level (1 byte) each</t>
   </si>
   <si>
-    <t>List of Pokemon it evolves into: Method (1 byte) target (2) method (2) forme target (1) number parameter (1)</t>
-  </si>
-  <si>
-    <t>List of evolves into it: source (2) forme (1) Method (1 byte) method (2)  number parameter (1)</t>
-  </si>
-  <si>
     <t>List of alt formes: forme # (1), method of transformation (1), item or move needed (2)</t>
   </si>
   <si>
@@ -255,6 +250,216 @@
   </si>
   <si>
     <t>bytes per entry frome here on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up with Friendship",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up at Morning with Friendship",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up at Night with Friendship",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Trade",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Trade with Held Item",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                $"Trade for opposite {specieslist[588]}/{specieslist[616]}", // Shelmet&amp;Karrablast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Used Item",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up (Attack &gt; Defense)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up (Attack = Defense)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up (Attack &lt; Defense)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up (Random &lt; 5)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up (Random &gt; 5)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                $"Level Up ({specieslist[291]})", // Ninjask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                $"Level Up ({specieslist[292]})", // Shedinja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up (Beauty)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Used Item (Male)", // Kirlia-&gt;Gallade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Used Item (Female)", // Snorunt-&gt;Froslass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up with Held Item (Day)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up with Held Item (Night)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up with Move",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up with Party",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up Male",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up Female",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up at Electric",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up at Forest",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up at Cold",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up with 3DS Upside Down",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up with 50 Affection + MoveType",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                $"{typelist[16]} Type in Party",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Overworld Rain",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up (@) at Morning",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up (@) at Night",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "Level Up Female (SetForm 1)",</t>
+  </si>
+  <si>
+    <t>Level Up</t>
+  </si>
+  <si>
+    <t>Trade</t>
+  </si>
+  <si>
+    <t>Trade with Held Item</t>
+  </si>
+  <si>
+    <t>Used Item</t>
+  </si>
+  <si>
+    <t>Level Up (Attack &gt; Defense)</t>
+  </si>
+  <si>
+    <t>Level Up (Attack = Defense)</t>
+  </si>
+  <si>
+    <t>Level Up (Attack &lt; Defense)</t>
+  </si>
+  <si>
+    <t>Level Up (Beauty)</t>
+  </si>
+  <si>
+    <t>Level Up with Move</t>
+  </si>
+  <si>
+    <t>Level Up Male</t>
+  </si>
+  <si>
+    <t>Level Up Female</t>
+  </si>
+  <si>
+    <t>Level Up at Electric</t>
+  </si>
+  <si>
+    <t>Level Up at Forest</t>
+  </si>
+  <si>
+    <t>Level Up at Cold</t>
+  </si>
+  <si>
+    <t>Level Up with 3DS Upside Down</t>
+  </si>
+  <si>
+    <t>Overworld Rain</t>
+  </si>
+  <si>
+    <t>Level Up (Friendship)</t>
+  </si>
+  <si>
+    <t>Level Up (Friendship, Night)</t>
+  </si>
+  <si>
+    <t>Level Up (Friendship, Day)</t>
+  </si>
+  <si>
+    <t>Trade Karrablast/Shelmet</t>
+  </si>
+  <si>
+    <t>Level Up (Encryption constant &lt;= 4)</t>
+  </si>
+  <si>
+    <t>Level Up (Encryption constant &gt;= 5)</t>
+  </si>
+  <si>
+    <t>Level Up (Branched Evolution, 1st)</t>
+  </si>
+  <si>
+    <t>Level Up (Branched Evolution, 2nd)</t>
+  </si>
+  <si>
+    <t>Used Item (Male)</t>
+  </si>
+  <si>
+    <t>Used Item (Female)</t>
+  </si>
+  <si>
+    <t>Level Up Holding Item (Day)</t>
+  </si>
+  <si>
+    <t>Level Up Holding Item (NIght)</t>
+  </si>
+  <si>
+    <t>Level Up with Pokemon</t>
+  </si>
+  <si>
+    <t>Level Up with 50 Affection + Move Type</t>
+  </si>
+  <si>
+    <t>Type in Party</t>
+  </si>
+  <si>
+    <t>Level Up (Morning)</t>
+  </si>
+  <si>
+    <t>Level Up (Night)</t>
+  </si>
+  <si>
+    <t>List of Pokemon it evolves into: Method (1 byte) target species (2) forme target (1) item/move parameter (2) number parameter (1)</t>
+  </si>
+  <si>
+    <t>List of evolves into it: Method (1 byte) target species (2) forme target (1) item/move parameter (2) number parameter (1)</t>
   </si>
 </sst>
 </file>
@@ -631,13 +836,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31FDE52E-1438-4E4D-B985-58AEBB556F45}">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="83.86328125" customWidth="1"/>
+    <col min="2" max="2" width="101.46484375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
@@ -653,7 +858,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -665,7 +870,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -677,7 +882,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -689,7 +894,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -701,7 +906,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -725,7 +930,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -737,7 +942,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1460,18 +1665,18 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C67">
         <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B68" t="s">
-        <v>61</v>
+        <v>139</v>
       </c>
       <c r="C68">
         <v>7</v>
@@ -1479,7 +1684,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B69" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="C69">
         <v>7</v>
@@ -1487,7 +1692,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B70" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C70">
         <v>4</v>
@@ -1499,6 +1704,441 @@
       </c>
       <c r="C71">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08AB0973-A846-4BA3-BEDA-C53E73ED6D9C}">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="65.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="str">
+        <f>TRIM(A1)</f>
+        <v>"",</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B35" si="0">TRIM(A2)</f>
+        <v>"Level Up with Friendship",</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up at Morning with Friendship",</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up at Night with Friendship",</v>
+      </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up",</v>
+      </c>
+      <c r="C5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>"Trade",</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>"Trade with Held Item",</v>
+      </c>
+      <c r="C7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>$"Trade for opposite {specieslist[588]}/{specieslist[616]}", // Shelmet&amp;Karrablast</v>
+      </c>
+      <c r="C8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>"Used Item",</v>
+      </c>
+      <c r="C9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up (Attack &gt; Defense)",</v>
+      </c>
+      <c r="C10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up (Attack = Defense)",</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up (Attack &lt; Defense)",</v>
+      </c>
+      <c r="C12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up (Random &lt; 5)",</v>
+      </c>
+      <c r="C13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up (Random &gt; 5)",</v>
+      </c>
+      <c r="C14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>$"Level Up ({specieslist[291]})", // Ninjask</v>
+      </c>
+      <c r="C15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>$"Level Up ({specieslist[292]})", // Shedinja</v>
+      </c>
+      <c r="C16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up (Beauty)",</v>
+      </c>
+      <c r="C17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>"Used Item (Male)", // Kirlia-&gt;Gallade</v>
+      </c>
+      <c r="C18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>"Used Item (Female)", // Snorunt-&gt;Froslass</v>
+      </c>
+      <c r="C19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up with Held Item (Day)",</v>
+      </c>
+      <c r="C20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up with Held Item (Night)",</v>
+      </c>
+      <c r="C21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up with Move",</v>
+      </c>
+      <c r="C22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up with Party",</v>
+      </c>
+      <c r="C23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up Male",</v>
+      </c>
+      <c r="C24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up Female",</v>
+      </c>
+      <c r="C25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up at Electric",</v>
+      </c>
+      <c r="C26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up at Forest",</v>
+      </c>
+      <c r="C27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up at Cold",</v>
+      </c>
+      <c r="C28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up with 3DS Upside Down",</v>
+      </c>
+      <c r="C29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up with 50 Affection + MoveType",</v>
+      </c>
+      <c r="C30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>$"{typelist[16]} Type in Party",</v>
+      </c>
+      <c r="C31" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>"Overworld Rain",</v>
+      </c>
+      <c r="C32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up (@) at Morning",</v>
+      </c>
+      <c r="C33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up (@) at Night",</v>
+      </c>
+      <c r="C34" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>"Level Up Female (SetForm 1)",</v>
+      </c>
+      <c r="C35" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>